<commit_message>
Se agrega botón para limpiar escaneados
</commit_message>
<xml_diff>
--- a/recuento_stock.xlsx
+++ b/recuento_stock.xlsx
@@ -448,21 +448,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ROPA001</t>
+          <t>BS-2DQRUSBWS</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BS-2DQRUSBWS</t>
+          <t>ROPA001</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integración de BD de Finnegans de productos
</commit_message>
<xml_diff>
--- a/recuento_stock.xlsx
+++ b/recuento_stock.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Nombre del Producto</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unidades</t>
         </is>
       </c>
@@ -448,21 +453,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BS-2DQRUSBWS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>8</v>
+          <t>ROPA001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BOTA PETROLERA-T 40-MARRON-MASC-BORIS C/CORDONES 3703 -21%</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ROPA001</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>9</v>
+          <t>ROPA007</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BOTA PETROLERA-T 38-MARRON-MASC-BORIS LOW LINE 3910X/3910D-21%</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ROPA009</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BOTA PETROLERA-T 40-MARRON-MASC-BORIS LOW LINE 3910X/3910D-21%</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ROPA123</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ZAPATO -T 38-MARRON-MASC-BORIS 3161D MD-21%</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ROPA112</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BOTIN -T 42-MARRON-MASC-FUNCIONAL TERRA BROWN-21%</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>